<commit_message>
added more, will be done by tonight
</commit_message>
<xml_diff>
--- a/flowering_time_merged_with-gene-interval.xlsx
+++ b/flowering_time_merged_with-gene-interval.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3397" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="490">
   <si>
     <t>Abrevation</t>
   </si>
@@ -1452,6 +1452,75 @@
   </si>
   <si>
     <t>Cytokinin-Deficient Transgenic Arabidopsis Plants Show Multiple Developmental Alterations Indicating Opposite Functions of Cytokinins in the Regulation of Shoot and Root Meristem Activity.</t>
+  </si>
+  <si>
+    <t>Transcriptomic Analysis of Arabidopsis Overexpressing Flowering Locus T Driven by a Meristem- Specific Promoter that Induces Early Flowering</t>
+  </si>
+  <si>
+    <t>Transcriptional regulation of LUX by CBF1 mediates cold input to the circadian clock in Arabidopsis</t>
+  </si>
+  <si>
+    <t>LUX ARRHYTHMO encodes a Myb domain protein essential for circadian rhythms.</t>
+  </si>
+  <si>
+    <t>A Phylogenomic Investigation of CYCLOIDEA-Like TCP Genes in the Leguminosae.</t>
+  </si>
+  <si>
+    <t>Phytochrome A null mutants of Arabidopsis display a wild-type phenotype in white light.</t>
+  </si>
+  <si>
+    <t>Rapid and Reversible Light-Mediated Chromatin Modifications of Arabidopsis Phytochrome A Locus</t>
+  </si>
+  <si>
+    <t>Sucrose control of phytochrome A signaling in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Genetic interactions between phytochrome A, phytochrome B, and cryptochrome 1 during Arabidopsis development.</t>
+  </si>
+  <si>
+    <t>The Protein Kinase SnRK2.6 Mediates the Regulation of Sucrose Metabolism and Plant Growth in Arabidopsis.</t>
+  </si>
+  <si>
+    <t>Three Arabidopsis SnRK2 Protein Kinases, SRK2D/SnRK2.2, SRK2E/SnRK2.6/OST1 and SRK2I/SnRK2.3 Involved in ABA-Signaling are Essential for the Control of Seed Development and Dormancy.</t>
+  </si>
+  <si>
+    <t>Overexpression of the phytochrome B gene from Arabidopsis thaliana increases plant growth and yield of cotton (Gossypium hirsutum)</t>
+  </si>
+  <si>
+    <t>Characterization of Circadian-Associated Pseudo-Response Regulators: I. Comparative Studies on a Series of Transgenic Lines Misexpressing Five Distinctive PRR Genes in Arabidopsis thaliana.</t>
+  </si>
+  <si>
+    <t>The common bean growth habit gene PvTFL1y is a functional homolog of Arabidopsis TFL1</t>
+  </si>
+  <si>
+    <t>Arabidopsis B-BOX32 interacts with CONSTANS-LIKE3 to regulate flowering</t>
+  </si>
+  <si>
+    <t>Analysis of the function of two circadian-regulated CONSTANS-LIKE genes.</t>
+  </si>
+  <si>
+    <t>Divergent Regulation of CBF Regulon on Cold Tolerance and Plant Phenotype in Cassava Overexpressing Arabidopsis CBF3 Gene</t>
+  </si>
+  <si>
+    <t>The cbfs triple mutants reveal the essential functions of CBFs in cold acclimation and allow the definition of CBF regulons in Arabidopsis</t>
+  </si>
+  <si>
+    <t>Mutational Evidence for the Critical Role of CBF Genes in Cold Acclimation in Arabidopsis</t>
+  </si>
+  <si>
+    <t>Overexpression of a phytochrome-regulated tandem zinc finger protein gene, OsTZF1, confers hypersensitivity to ABA and hyposensitivity to red light and far-red light in rice seedlings</t>
+  </si>
+  <si>
+    <t>Overexpressed phytochrome C has similar photosensory specificity to phytochrome B but a distinctive capacity to enhance primary leaf expansion.</t>
+  </si>
+  <si>
+    <t>Phytochrome C plays a major role in the acceleration of wheat flowering under long-day photoperiod</t>
+  </si>
+  <si>
+    <t>Arabidopsis phytochromes C and E have different spectral characteristics from those of phytochromes A and B.</t>
+  </si>
+  <si>
+    <t>Comparative functional analysis of full-length and N-terminal fragments of phytochrome C, D and E in red light-induced signaling</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1831,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1960,6 +2029,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2335,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.6875" defaultRowHeight="15.4"/>
@@ -2349,7 +2421,7 @@
     <col min="13" max="13" width="25.1875" style="1" customWidth="1"/>
     <col min="14" max="14" width="22.3125" style="1" customWidth="1"/>
     <col min="15" max="20" width="17.6875" style="1"/>
-    <col min="21" max="21" width="38.3125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="78.25" style="1" customWidth="1"/>
     <col min="22" max="22" width="20.625" style="1" customWidth="1"/>
     <col min="23" max="16384" width="17.6875" style="1"/>
   </cols>
@@ -5574,6 +5646,12 @@
       <c r="S52" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="T52" s="69">
+        <v>27154816</v>
+      </c>
+      <c r="U52" s="68" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="53" spans="1:21" ht="15.75">
       <c r="A53" s="2" t="s">
@@ -5639,7 +5717,7 @@
       <c r="B54" s="40" t="s">
         <v>357</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="68" t="s">
         <v>356</v>
       </c>
       <c r="D54" s="40" t="s">
@@ -5688,7 +5766,12 @@
       <c r="S54" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T54" s="1"/>
+      <c r="T54" s="69">
+        <v>24954045</v>
+      </c>
+      <c r="U54" s="71" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="55" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A55" s="15" t="s">
@@ -5748,7 +5831,12 @@
       <c r="S55" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T55" s="1"/>
+      <c r="T55" s="67">
+        <v>16006522</v>
+      </c>
+      <c r="U55" s="70" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="56" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A56" s="15" t="s">
@@ -5866,7 +5954,12 @@
       <c r="S57" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T57" s="1"/>
+      <c r="T57" s="69">
+        <v>12644657</v>
+      </c>
+      <c r="U57" s="76" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="58" spans="1:21" ht="15.75">
       <c r="A58" s="5" t="s">
@@ -5980,6 +6073,12 @@
       <c r="S59" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="T59" s="69">
+        <v>8364355</v>
+      </c>
+      <c r="U59" s="68" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="60" spans="1:21" ht="19.05" customHeight="1">
       <c r="A60" s="1" t="s">
@@ -6039,6 +6138,12 @@
       <c r="S60" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="T60" s="69">
+        <v>21317377</v>
+      </c>
+      <c r="U60" s="68" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="61" spans="1:21" s="18" customFormat="1" ht="20" customHeight="1">
       <c r="A61" s="1" t="s">
@@ -6098,10 +6203,15 @@
       <c r="S61" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T61" s="1"/>
+      <c r="T61" s="69">
+        <v>9144963</v>
+      </c>
+      <c r="U61" s="76" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="62" spans="1:21" s="18" customFormat="1" ht="20" customHeight="1">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="71" t="s">
         <v>144</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -6156,7 +6266,12 @@
       <c r="S62" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T62" s="1"/>
+      <c r="T62" s="67">
+        <v>9733523</v>
+      </c>
+      <c r="U62" s="76" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="63" spans="1:21" s="18" customFormat="1" ht="20" customHeight="1">
       <c r="A63" s="18" t="s">
@@ -6216,7 +6331,12 @@
       <c r="S63" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T63" s="1"/>
+      <c r="T63" s="67">
+        <v>20200070</v>
+      </c>
+      <c r="U63" s="76" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="64" spans="1:21" ht="18" customHeight="1">
       <c r="A64" s="1" t="s">
@@ -6276,8 +6396,14 @@
       <c r="S64" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T64" s="69">
+        <v>19541597</v>
+      </c>
+      <c r="U64" s="68" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A65" s="2" t="s">
         <v>228</v>
       </c>
@@ -6334,7 +6460,7 @@
       </c>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="66" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A66" s="2" t="s">
         <v>228</v>
       </c>
@@ -6391,7 +6517,7 @@
       </c>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="67" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A67" s="40" t="s">
         <v>352</v>
       </c>
@@ -6448,7 +6574,7 @@
       </c>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="68" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A68" s="5" t="s">
         <v>249</v>
       </c>
@@ -6503,10 +6629,15 @@
       <c r="S68" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T68" s="1"/>
-    </row>
-    <row r="69" spans="1:20" ht="15.75">
-      <c r="A69" s="2" t="s">
+      <c r="T68" s="69">
+        <v>11851908</v>
+      </c>
+      <c r="U68" s="71" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="15.75">
+      <c r="A69" s="71" t="s">
         <v>130</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -6561,8 +6692,14 @@
       <c r="S69" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" s="18" customFormat="1" ht="15.75">
+      <c r="T69" s="74">
+        <v>21462389</v>
+      </c>
+      <c r="U69" s="68" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" s="18" customFormat="1" ht="15.75">
       <c r="A70" s="15" t="s">
         <v>231</v>
       </c>
@@ -6620,9 +6757,14 @@
       <c r="S70" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T70" s="1"/>
-    </row>
-    <row r="71" spans="1:20" ht="15.75">
+      <c r="T70" s="69">
+        <v>17284849</v>
+      </c>
+      <c r="U70" s="76" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="15.75">
       <c r="A71" s="17" t="s">
         <v>215</v>
       </c>
@@ -6681,7 +6823,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="72" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="72" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A72" s="17" t="s">
         <v>215</v>
       </c>
@@ -6741,7 +6883,7 @@
       </c>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="73" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -6801,7 +6943,7 @@
       </c>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="74" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A74" s="2" t="s">
         <v>161</v>
       </c>
@@ -6856,9 +6998,14 @@
       <c r="S74" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T74" s="1"/>
-    </row>
-    <row r="75" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T74" s="69">
+        <v>22331140</v>
+      </c>
+      <c r="U74" s="71" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A75" s="2" t="s">
         <v>226</v>
       </c>
@@ -6915,7 +7062,7 @@
       </c>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" s="2" customFormat="1">
+    <row r="76" spans="1:21" s="2" customFormat="1">
       <c r="A76" s="2" t="s">
         <v>55</v>
       </c>
@@ -6970,9 +7117,14 @@
       <c r="S76" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T76" s="1"/>
-    </row>
-    <row r="77" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T76" s="69">
+        <v>27999181</v>
+      </c>
+      <c r="U76" s="71" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A77" s="2" t="s">
         <v>55</v>
       </c>
@@ -7027,9 +7179,14 @@
       <c r="S77" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T77" s="1"/>
-    </row>
-    <row r="78" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T77" s="69">
+        <v>11359606</v>
+      </c>
+      <c r="U77" s="71" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A78" s="1" t="s">
         <v>375</v>
       </c>
@@ -7084,9 +7241,14 @@
       <c r="S78" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T78" s="1"/>
-    </row>
-    <row r="79" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T78" s="67">
+        <v>27999588</v>
+      </c>
+      <c r="U78" s="71" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A79" s="1" t="s">
         <v>375</v>
       </c>
@@ -7141,9 +7303,14 @@
       <c r="S79" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T79" s="1"/>
-    </row>
-    <row r="80" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T79" s="69">
+        <v>27353960</v>
+      </c>
+      <c r="U79" s="71" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A80" s="1" t="s">
         <v>375</v>
       </c>
@@ -7199,9 +7366,14 @@
       <c r="S80" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T80" s="1"/>
-    </row>
-    <row r="81" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T80" s="69">
+        <v>27252305</v>
+      </c>
+      <c r="U80" s="71" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A81" s="43" t="s">
         <v>349</v>
       </c>
@@ -7261,7 +7433,7 @@
       </c>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" s="15" customFormat="1" ht="15.75">
+    <row r="82" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A82" s="15" t="s">
         <v>233</v>
       </c>
@@ -7321,7 +7493,7 @@
       </c>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" s="52" customFormat="1" ht="15.75">
+    <row r="83" spans="1:21" s="52" customFormat="1" ht="15.75">
       <c r="A83" s="44" t="s">
         <v>151</v>
       </c>
@@ -7377,9 +7549,14 @@
       <c r="S83" s="44" t="s">
         <v>419</v>
       </c>
-      <c r="T83" s="44"/>
-    </row>
-    <row r="84" spans="1:20" s="2" customFormat="1" ht="15.75">
+      <c r="T83" s="69">
+        <v>22572927</v>
+      </c>
+      <c r="U83" s="77" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A84" s="1" t="s">
         <v>151</v>
       </c>
@@ -7435,9 +7612,14 @@
       <c r="S84" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T84" s="1"/>
-    </row>
-    <row r="85" spans="1:20" s="15" customFormat="1" ht="15.75">
+      <c r="T84" s="69">
+        <v>9418054</v>
+      </c>
+      <c r="U84" s="71" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A85" s="18" t="s">
         <v>151</v>
       </c>
@@ -7495,9 +7677,14 @@
       <c r="S85" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T85" s="1"/>
-    </row>
-    <row r="86" spans="1:20" s="15" customFormat="1" ht="15.75">
+      <c r="T85" s="74">
+        <v>24961368</v>
+      </c>
+      <c r="U85" s="70" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A86" s="18" t="s">
         <v>151</v>
       </c>
@@ -7555,9 +7742,14 @@
       <c r="S86" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T86" s="1"/>
-    </row>
-    <row r="87" spans="1:20" s="15" customFormat="1" ht="15.75">
+      <c r="T86" s="69">
+        <v>10734217</v>
+      </c>
+      <c r="U86" s="70" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A87" s="18" t="s">
         <v>151</v>
       </c>
@@ -7615,9 +7807,14 @@
       <c r="S87" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T87" s="1"/>
-    </row>
-    <row r="88" spans="1:20" s="44" customFormat="1">
+      <c r="T87" s="67">
+        <v>23772959</v>
+      </c>
+      <c r="U87" s="70" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" s="44" customFormat="1">
       <c r="A88" s="59" t="s">
         <v>28</v>
       </c>
@@ -7673,7 +7870,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="18" customFormat="1">
+    <row r="89" spans="1:21" s="18" customFormat="1">
       <c r="A89" s="20" t="s">
         <v>28</v>
       </c>
@@ -7733,7 +7930,7 @@
       </c>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" s="18" customFormat="1">
+    <row r="90" spans="1:21" s="18" customFormat="1">
       <c r="A90" s="20" t="s">
         <v>28</v>
       </c>
@@ -7793,7 +7990,7 @@
       </c>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" s="18" customFormat="1">
+    <row r="91" spans="1:21" s="18" customFormat="1">
       <c r="A91" s="20" t="s">
         <v>28</v>
       </c>
@@ -7853,7 +8050,7 @@
       </c>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" s="2" customFormat="1">
+    <row r="92" spans="1:21" s="2" customFormat="1">
       <c r="A92" s="4" t="s">
         <v>28</v>
       </c>
@@ -7911,7 +8108,7 @@
       </c>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" s="15" customFormat="1" ht="15.75">
+    <row r="93" spans="1:21" s="15" customFormat="1" ht="15.75">
       <c r="A93" s="1" t="s">
         <v>153</v>
       </c>
@@ -7969,7 +8166,7 @@
       </c>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="94" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A94" s="1" t="s">
         <v>153</v>
       </c>
@@ -8029,7 +8226,7 @@
       </c>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" s="2" customFormat="1" ht="15.75">
+    <row r="95" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A95" s="1" t="s">
         <v>153</v>
       </c>
@@ -8089,7 +8286,7 @@
       </c>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:21">
       <c r="A96" s="1" t="s">
         <v>165</v>
       </c>
@@ -11223,9 +11420,33 @@
     <hyperlink ref="T48" r:id="rId39" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21069430&amp;dopt=Abstract"/>
     <hyperlink ref="T50" r:id="rId40" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27072125&amp;dopt=Abstract"/>
     <hyperlink ref="T51" r:id="rId41" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14555694&amp;dopt=Abstract"/>
+    <hyperlink ref="T52" r:id="rId42" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27154816&amp;dopt=Abstract"/>
+    <hyperlink ref="T54" r:id="rId43" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24954045&amp;dopt=Abstract"/>
+    <hyperlink ref="T55" r:id="rId44" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16006522&amp;dopt=Abstract"/>
+    <hyperlink ref="T57" r:id="rId45" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12644657&amp;dopt=Abstract"/>
+    <hyperlink ref="T59" r:id="rId46" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=8364355&amp;dopt=Abstract"/>
+    <hyperlink ref="T60" r:id="rId47" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21317377&amp;dopt=Abstract"/>
+    <hyperlink ref="T61" r:id="rId48" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9144963&amp;dopt=Abstract"/>
+    <hyperlink ref="T62" r:id="rId49" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9733523&amp;dopt=Abstract"/>
+    <hyperlink ref="T63" r:id="rId50" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20200070&amp;dopt=Abstract"/>
+    <hyperlink ref="T64" r:id="rId51" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19541597&amp;dopt=Abstract"/>
+    <hyperlink ref="T68" r:id="rId52" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11851908&amp;dopt=Abstract"/>
+    <hyperlink ref="T69" r:id="rId53" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21462389&amp;dopt=Abstract"/>
+    <hyperlink ref="T70" r:id="rId54" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17284849&amp;dopt=Abstract"/>
+    <hyperlink ref="T74" r:id="rId55" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22331140&amp;dopt=Abstract"/>
+    <hyperlink ref="T76" r:id="rId56" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999181&amp;dopt=Abstract"/>
+    <hyperlink ref="T77" r:id="rId57" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11359606&amp;dopt=Abstract"/>
+    <hyperlink ref="T78" r:id="rId58" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999588&amp;dopt=Abstract"/>
+    <hyperlink ref="T79" r:id="rId59" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27353960&amp;dopt=Abstract"/>
+    <hyperlink ref="T80" r:id="rId60" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27252305&amp;dopt=Abstract"/>
+    <hyperlink ref="T83" r:id="rId61" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22572927&amp;dopt=Abstract"/>
+    <hyperlink ref="T84" r:id="rId62" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9418054&amp;dopt=Abstract"/>
+    <hyperlink ref="T85" r:id="rId63" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24961368&amp;dopt=Abstract"/>
+    <hyperlink ref="T86" r:id="rId64" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10734217&amp;dopt=Abstract"/>
+    <hyperlink ref="T87" r:id="rId65" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23772959&amp;dopt=Abstract"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId42"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId66"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
searched Barley and rice.
</commit_message>
<xml_diff>
--- a/flowering_time_merged_with-gene-interval.xlsx
+++ b/flowering_time_merged_with-gene-interval.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="532">
   <si>
     <t>Abrevation</t>
   </si>
@@ -1590,6 +1590,63 @@
   </si>
   <si>
     <t>The 5'UTR of CCA1 includes an autoregulatory cis element that segregates between light and circadian regulation of CCA1 and LHY</t>
+  </si>
+  <si>
+    <t>PMC2806734</t>
+  </si>
+  <si>
+    <t>Cleistogamous flowering in barley arises from the suppression of microRNA-guided HvAP2 mRNA cleavage.</t>
+  </si>
+  <si>
+    <t>Genome dynamics explain the evolution of flowering time CCT domain gene families in the Poaceae.</t>
+  </si>
+  <si>
+    <t>Six-rowed barley originated from a mutation in a homeodomain-leucine zipper I-class homeobox gene.</t>
+  </si>
+  <si>
+    <t>Evolution of the Grain Dispersal System in Barley</t>
+  </si>
+  <si>
+    <t>HvLUX1 is a candidate gene underlying the early maturity 10 locus in barley: phylogeny, diversity, and interactions with the circadian clock and photoperiodic pathways.</t>
+  </si>
+  <si>
+    <t>Phytochrome C is a key factor controlling long-day flowering in barley.</t>
+  </si>
+  <si>
+    <t>Low temperatures induce rapid changes in chromatin state and transcript levels of the cereal VERNALIZATION1 gene.</t>
+  </si>
+  <si>
+    <t>The promoter of the cereal VERNALIZATION1 gene is sufficient for transcriptional induction by prolonged cold.</t>
+  </si>
+  <si>
+    <t>Positional relationships between photoperiod response QTL and photoreceptor and vernalization genes in barley.</t>
+  </si>
+  <si>
+    <t>Haplotype analysis of vernalization loci in European barley germplasm reveals novel VRN-H1 alleles and a predominant winter VRN-H1/VRN-H2 multi-locus haplotype.</t>
+  </si>
+  <si>
+    <t>Regions associated with repression of the barley (Hordeum vulgare) VERNALIZATION1 gene are not required for cold induction.</t>
+  </si>
+  <si>
+    <t>Molecular and structural characterization of barley vernalization genes.</t>
+  </si>
+  <si>
+    <t>Detection of DNA Methylation in Hd1, Hd3a, and Hd6 Genes in Rice KDML 105 (Oryza sativa L.)</t>
+  </si>
+  <si>
+    <t>Unpublished</t>
+  </si>
+  <si>
+    <t>The evolution of CONSTANS-like gene families in barley, rice, and Arabidopsis.</t>
+  </si>
+  <si>
+    <t>The altered pattern of amylose accumulation in the endosperm of low-amylose barley cultivars is attributable to a single mutant allele of granule-bound starch synthase I with a deletion in the 5'-non-coding region.</t>
+  </si>
+  <si>
+    <t>Genome-wide SNPs and re-sequencing of growth habit and inflorescence genes in barley: implications for association mapping in germplasm arrays varying in size and structure.</t>
+  </si>
+  <si>
+    <t>Barley grain with adhering hulls is controlled by an ERF family transcription factor gene regulating a lipid biosynthesis pathway</t>
   </si>
 </sst>
 </file>
@@ -1900,7 +1957,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2105,6 +2162,24 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="92">
@@ -2479,7 +2554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
@@ -2618,6 +2693,12 @@
       <c r="S2" s="2" t="s">
         <v>419</v>
       </c>
+      <c r="T2" s="80">
+        <v>23028921</v>
+      </c>
+      <c r="U2" s="71" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="5" t="s">
@@ -5130,7 +5211,7 @@
       <c r="A43" s="44" t="s">
         <v>363</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="81" t="s">
         <v>363</v>
       </c>
       <c r="C43" s="44" t="s">
@@ -5180,6 +5261,12 @@
       </c>
       <c r="S43" s="44" t="s">
         <v>419</v>
+      </c>
+      <c r="T43" s="82">
+        <v>17220272</v>
+      </c>
+      <c r="U43" s="81" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="44" spans="1:21" s="2" customFormat="1" ht="15.75">
@@ -5359,7 +5446,12 @@
       <c r="S46" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T46" s="1"/>
+      <c r="T46" s="79" t="s">
+        <v>513</v>
+      </c>
+      <c r="U46" s="71" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="47" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A47" s="2" t="s">
@@ -5535,7 +5627,12 @@
       <c r="S49" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T49" s="1"/>
+      <c r="T49" s="80">
+        <v>26232223</v>
+      </c>
+      <c r="U49" s="71" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="50" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A50" s="2" t="s">
@@ -5968,7 +6065,12 @@
       <c r="S56" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T56" s="1"/>
+      <c r="T56" s="83">
+        <v>23731278</v>
+      </c>
+      <c r="U56" s="70" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="57" spans="1:21" s="18" customFormat="1" ht="15.75">
       <c r="A57" s="1" t="s">
@@ -7941,6 +8043,12 @@
       <c r="S88" s="44" t="s">
         <v>419</v>
       </c>
+      <c r="T88" s="82">
+        <v>24014575</v>
+      </c>
+      <c r="U88" s="81" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="89" spans="1:21" s="18" customFormat="1">
       <c r="A89" s="20" t="s">
@@ -8236,7 +8344,12 @@
       <c r="S93" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T93" s="1"/>
+      <c r="T93" s="83">
+        <v>23580755</v>
+      </c>
+      <c r="U93" s="70" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="94" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A94" s="1" t="s">
@@ -8296,7 +8409,12 @@
       <c r="S94" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T94" s="1"/>
+      <c r="T94" s="83">
+        <v>22242122</v>
+      </c>
+      <c r="U94" s="71" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="95" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A95" s="1" t="s">
@@ -8356,7 +8474,12 @@
       <c r="S95" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T95" s="1"/>
+      <c r="T95" s="80">
+        <v>16489429</v>
+      </c>
+      <c r="U95" s="71" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="96" spans="1:21">
       <c r="A96" s="1" t="s">
@@ -8413,8 +8536,14 @@
       <c r="S96" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" s="18" customFormat="1">
+      <c r="T96" s="80">
+        <v>17713756</v>
+      </c>
+      <c r="U96" s="68" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" s="18" customFormat="1" ht="30.75">
       <c r="A97" s="18" t="s">
         <v>165</v>
       </c>
@@ -8472,7 +8601,12 @@
       <c r="S97" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T97" s="1"/>
+      <c r="T97" s="83">
+        <v>19404679</v>
+      </c>
+      <c r="U97" s="84" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="98" spans="1:21" s="18" customFormat="1">
       <c r="A98" s="18" t="s">
@@ -8590,7 +8724,12 @@
       <c r="S99" s="44" t="s">
         <v>419</v>
       </c>
-      <c r="T99" s="44"/>
+      <c r="T99" s="80">
+        <v>16235110</v>
+      </c>
+      <c r="U99" s="77" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="100" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A100" s="2" t="s">
@@ -8647,7 +8786,12 @@
       <c r="S100" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T100" s="1"/>
+      <c r="T100" s="68" t="s">
+        <v>527</v>
+      </c>
+      <c r="U100" s="71" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="101" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A101" s="2" t="s">
@@ -8762,7 +8906,12 @@
       <c r="S102" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T102" s="1"/>
+      <c r="T102" s="80">
+        <v>12692345</v>
+      </c>
+      <c r="U102" s="70" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="103" spans="1:21" s="15" customFormat="1">
       <c r="A103" s="5" t="s">
@@ -9764,7 +9913,12 @@
       <c r="S118" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T118" s="1"/>
+      <c r="T118" s="80">
+        <v>12226499</v>
+      </c>
+      <c r="U118" s="70" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="119" spans="1:21" s="2" customFormat="1" ht="15.75">
       <c r="A119" s="1" t="s">
@@ -10267,7 +10421,12 @@
       <c r="S126" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T126" s="1"/>
+      <c r="T126" s="80">
+        <v>21159198</v>
+      </c>
+      <c r="U126" s="76" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="127" spans="1:21" s="18" customFormat="1" ht="15.75">
       <c r="A127" s="18" t="s">
@@ -11107,12 +11266,18 @@
       <c r="S140" s="1" t="s">
         <v>419</v>
       </c>
+      <c r="T140" s="80">
+        <v>18316719</v>
+      </c>
+      <c r="U140" s="68" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="141" spans="1:21" ht="15.75">
       <c r="A141" s="40" t="s">
         <v>378</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="68" t="s">
         <v>379</v>
       </c>
       <c r="C141" s="1" t="s">
@@ -11622,63 +11787,79 @@
     <hyperlink ref="T40" r:id="rId35" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16428600&amp;dopt=Abstract"/>
     <hyperlink ref="T41" r:id="rId36" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26136262&amp;dopt=Abstract"/>
     <hyperlink ref="T42" r:id="rId37" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22564282&amp;dopt=Abstract"/>
-    <hyperlink ref="T44" r:id="rId38" display="https://www.ncbi.nlm.nih.gov/pubmed/9482818"/>
-    <hyperlink ref="T48" r:id="rId39" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21069430&amp;dopt=Abstract"/>
-    <hyperlink ref="T50" r:id="rId40" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27072125&amp;dopt=Abstract"/>
-    <hyperlink ref="T51" r:id="rId41" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14555694&amp;dopt=Abstract"/>
-    <hyperlink ref="T52" r:id="rId42" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27154816&amp;dopt=Abstract"/>
-    <hyperlink ref="T54" r:id="rId43" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24954045&amp;dopt=Abstract"/>
-    <hyperlink ref="T55" r:id="rId44" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16006522&amp;dopt=Abstract"/>
-    <hyperlink ref="T57" r:id="rId45" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12644657&amp;dopt=Abstract"/>
-    <hyperlink ref="T59" r:id="rId46" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=8364355&amp;dopt=Abstract"/>
-    <hyperlink ref="T60" r:id="rId47" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21317377&amp;dopt=Abstract"/>
-    <hyperlink ref="T61" r:id="rId48" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9144963&amp;dopt=Abstract"/>
-    <hyperlink ref="T62" r:id="rId49" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9733523&amp;dopt=Abstract"/>
-    <hyperlink ref="T63" r:id="rId50" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20200070&amp;dopt=Abstract"/>
-    <hyperlink ref="T64" r:id="rId51" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19541597&amp;dopt=Abstract"/>
-    <hyperlink ref="T68" r:id="rId52" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11851908&amp;dopt=Abstract"/>
-    <hyperlink ref="T69" r:id="rId53" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21462389&amp;dopt=Abstract"/>
-    <hyperlink ref="T70" r:id="rId54" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17284849&amp;dopt=Abstract"/>
-    <hyperlink ref="T74" r:id="rId55" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22331140&amp;dopt=Abstract"/>
-    <hyperlink ref="T76" r:id="rId56" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999181&amp;dopt=Abstract"/>
-    <hyperlink ref="T77" r:id="rId57" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11359606&amp;dopt=Abstract"/>
-    <hyperlink ref="T78" r:id="rId58" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999588&amp;dopt=Abstract"/>
-    <hyperlink ref="T79" r:id="rId59" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27353960&amp;dopt=Abstract"/>
-    <hyperlink ref="T80" r:id="rId60" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27252305&amp;dopt=Abstract"/>
-    <hyperlink ref="T83" r:id="rId61" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22572927&amp;dopt=Abstract"/>
-    <hyperlink ref="T84" r:id="rId62" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9418054&amp;dopt=Abstract"/>
-    <hyperlink ref="T85" r:id="rId63" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24961368&amp;dopt=Abstract"/>
-    <hyperlink ref="T86" r:id="rId64" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10734217&amp;dopt=Abstract"/>
-    <hyperlink ref="T87" r:id="rId65" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23772959&amp;dopt=Abstract"/>
-    <hyperlink ref="T103" r:id="rId66" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17478635&amp;dopt=Abstract"/>
-    <hyperlink ref="T104" r:id="rId67" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26810763&amp;dopt=Abstract"/>
-    <hyperlink ref="T105" r:id="rId68" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19504268&amp;dopt=Abstract"/>
-    <hyperlink ref="T106" r:id="rId69" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19816401&amp;dopt=Abstract"/>
-    <hyperlink ref="T107" r:id="rId70" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11828023&amp;dopt=Abstract"/>
-    <hyperlink ref="T108" r:id="rId71" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14605222&amp;dopt=Abstract"/>
-    <hyperlink ref="T109" r:id="rId72" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16703358&amp;dopt=Abstract"/>
-    <hyperlink ref="T110" r:id="rId73" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17259260&amp;dopt=Abstract"/>
-    <hyperlink ref="T112" r:id="rId74" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11359606&amp;dopt=Abstract"/>
-    <hyperlink ref="T113" r:id="rId75" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23265320&amp;dopt=Abstract"/>
-    <hyperlink ref="T115" r:id="rId76" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25710501&amp;dopt=Abstract"/>
-    <hyperlink ref="T116" r:id="rId77" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12777053&amp;dopt=Abstract"/>
-    <hyperlink ref="T117" r:id="rId78" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25630334&amp;dopt=Abstract"/>
-    <hyperlink ref="T119" r:id="rId79" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21890645&amp;dopt=Abstract"/>
-    <hyperlink ref="T120" r:id="rId80" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17446353&amp;dopt=Abstract"/>
-    <hyperlink ref="T121" r:id="rId81" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10583961&amp;dopt=Abstract"/>
-    <hyperlink ref="T122" r:id="rId82" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23607279&amp;dopt=Abstract"/>
-    <hyperlink ref="T123" r:id="rId83" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26212862&amp;dopt=Abstract"/>
-    <hyperlink ref="T124" r:id="rId84" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19656342&amp;dopt=Abstract"/>
-    <hyperlink ref="T125" r:id="rId85" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23563564&amp;dopt=Abstract"/>
-    <hyperlink ref="T129" r:id="rId86" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17257168&amp;dopt=Abstract"/>
-    <hyperlink ref="T131" r:id="rId87" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19566593&amp;dopt=Abstract"/>
-    <hyperlink ref="T132" r:id="rId88" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23265320&amp;dopt=Abstract"/>
-    <hyperlink ref="T134" r:id="rId89" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23027948&amp;dopt=Abstract"/>
-    <hyperlink ref="T135" r:id="rId90" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21781194&amp;dopt=Abstract"/>
-    <hyperlink ref="T136" r:id="rId91" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20119844&amp;dopt=Abstract"/>
+    <hyperlink ref="T48" r:id="rId38" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21069430&amp;dopt=Abstract"/>
+    <hyperlink ref="T50" r:id="rId39" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27072125&amp;dopt=Abstract"/>
+    <hyperlink ref="T51" r:id="rId40" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14555694&amp;dopt=Abstract"/>
+    <hyperlink ref="T52" r:id="rId41" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27154816&amp;dopt=Abstract"/>
+    <hyperlink ref="T54" r:id="rId42" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24954045&amp;dopt=Abstract"/>
+    <hyperlink ref="T55" r:id="rId43" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16006522&amp;dopt=Abstract"/>
+    <hyperlink ref="T59" r:id="rId44" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=8364355&amp;dopt=Abstract"/>
+    <hyperlink ref="T60" r:id="rId45" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21317377&amp;dopt=Abstract"/>
+    <hyperlink ref="T61" r:id="rId46" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9144963&amp;dopt=Abstract"/>
+    <hyperlink ref="T62" r:id="rId47" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9733523&amp;dopt=Abstract"/>
+    <hyperlink ref="T63" r:id="rId48" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20200070&amp;dopt=Abstract"/>
+    <hyperlink ref="T64" r:id="rId49" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19541597&amp;dopt=Abstract"/>
+    <hyperlink ref="T68" r:id="rId50" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11851908&amp;dopt=Abstract"/>
+    <hyperlink ref="T69" r:id="rId51" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21462389&amp;dopt=Abstract"/>
+    <hyperlink ref="T70" r:id="rId52" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17284849&amp;dopt=Abstract"/>
+    <hyperlink ref="T74" r:id="rId53" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22331140&amp;dopt=Abstract"/>
+    <hyperlink ref="T76" r:id="rId54" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999181&amp;dopt=Abstract"/>
+    <hyperlink ref="T77" r:id="rId55" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11359606&amp;dopt=Abstract"/>
+    <hyperlink ref="T78" r:id="rId56" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27999588&amp;dopt=Abstract"/>
+    <hyperlink ref="T79" r:id="rId57" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27353960&amp;dopt=Abstract"/>
+    <hyperlink ref="T80" r:id="rId58" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=27252305&amp;dopt=Abstract"/>
+    <hyperlink ref="T83" r:id="rId59" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=22572927&amp;dopt=Abstract"/>
+    <hyperlink ref="T84" r:id="rId60" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=9418054&amp;dopt=Abstract"/>
+    <hyperlink ref="T85" r:id="rId61" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=24961368&amp;dopt=Abstract"/>
+    <hyperlink ref="T86" r:id="rId62" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10734217&amp;dopt=Abstract"/>
+    <hyperlink ref="T87" r:id="rId63" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23772959&amp;dopt=Abstract"/>
+    <hyperlink ref="T103" r:id="rId64" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17478635&amp;dopt=Abstract"/>
+    <hyperlink ref="T104" r:id="rId65" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26810763&amp;dopt=Abstract"/>
+    <hyperlink ref="T105" r:id="rId66" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19504268&amp;dopt=Abstract"/>
+    <hyperlink ref="T106" r:id="rId67" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19816401&amp;dopt=Abstract"/>
+    <hyperlink ref="T107" r:id="rId68" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11828023&amp;dopt=Abstract"/>
+    <hyperlink ref="T108" r:id="rId69" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=14605222&amp;dopt=Abstract"/>
+    <hyperlink ref="T109" r:id="rId70" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=16703358&amp;dopt=Abstract"/>
+    <hyperlink ref="T110" r:id="rId71" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17259260&amp;dopt=Abstract"/>
+    <hyperlink ref="T112" r:id="rId72" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=11359606&amp;dopt=Abstract"/>
+    <hyperlink ref="T113" r:id="rId73" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23265320&amp;dopt=Abstract"/>
+    <hyperlink ref="T115" r:id="rId74" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25710501&amp;dopt=Abstract"/>
+    <hyperlink ref="T116" r:id="rId75" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12777053&amp;dopt=Abstract"/>
+    <hyperlink ref="T117" r:id="rId76" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=25630334&amp;dopt=Abstract"/>
+    <hyperlink ref="T119" r:id="rId77" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21890645&amp;dopt=Abstract"/>
+    <hyperlink ref="T120" r:id="rId78" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17446353&amp;dopt=Abstract"/>
+    <hyperlink ref="T121" r:id="rId79" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=10583961&amp;dopt=Abstract"/>
+    <hyperlink ref="T122" r:id="rId80" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23607279&amp;dopt=Abstract"/>
+    <hyperlink ref="T123" r:id="rId81" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=26212862&amp;dopt=Abstract"/>
+    <hyperlink ref="T124" r:id="rId82" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19656342&amp;dopt=Abstract"/>
+    <hyperlink ref="T125" r:id="rId83" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23563564&amp;dopt=Abstract"/>
+    <hyperlink ref="T129" r:id="rId84" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=17257168&amp;dopt=Abstract"/>
+    <hyperlink ref="T131" r:id="rId85" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=19566593&amp;dopt=Abstract"/>
+    <hyperlink ref="T132" r:id="rId86" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23265320&amp;dopt=Abstract"/>
+    <hyperlink ref="T134" r:id="rId87" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=23027948&amp;dopt=Abstract"/>
+    <hyperlink ref="T135" r:id="rId88" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=21781194&amp;dopt=Abstract"/>
+    <hyperlink ref="T136" r:id="rId89" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=20119844&amp;dopt=Abstract"/>
+    <hyperlink ref="T46" r:id="rId90" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2806734/"/>
+    <hyperlink ref="T2" r:id="rId91" display="https://www.ncbi.nlm.nih.gov/pubmed/23028921"/>
+    <hyperlink ref="T44" r:id="rId92" display="https://www.ncbi.nlm.nih.gov/pubmed/9482818"/>
+    <hyperlink ref="T43" r:id="rId93" display="https://www.ncbi.nlm.nih.gov/pubmed/17220272"/>
+    <hyperlink ref="T49" r:id="rId94" display="https://www.ncbi.nlm.nih.gov/pubmed/26232223"/>
+    <hyperlink ref="T57" r:id="rId95" display="http://www.ncbi.nlm.nih.gov/entrez/query.fcgi?cmd=Retrieve&amp;db=PubMed&amp;list_uids=12644657&amp;dopt=Abstract"/>
+    <hyperlink ref="T56" r:id="rId96" display="https://www.ncbi.nlm.nih.gov/pubmed?LinkName=nuccore_pubmed&amp;from_uid=529158032"/>
+    <hyperlink ref="T88" r:id="rId97" display="https://www.ncbi.nlm.nih.gov/pubmed/24014575"/>
+    <hyperlink ref="T93" r:id="rId98" display="https://www.ncbi.nlm.nih.gov/pubmed/23580755"/>
+    <hyperlink ref="T94" r:id="rId99" display="https://www.ncbi.nlm.nih.gov/pubmed/22242122"/>
+    <hyperlink ref="T95" r:id="rId100" display="https://www.ncbi.nlm.nih.gov/pubmed/16489429"/>
+    <hyperlink ref="T96" r:id="rId101" display="https://www.ncbi.nlm.nih.gov/pubmed/17713756"/>
+    <hyperlink ref="T97" r:id="rId102" display="https://www.ncbi.nlm.nih.gov/pubmed/19404679"/>
+    <hyperlink ref="T99" r:id="rId103" display="https://www.ncbi.nlm.nih.gov/pubmed/16235110"/>
+    <hyperlink ref="T102" r:id="rId104" display="https://www.ncbi.nlm.nih.gov/pubmed/12692345"/>
+    <hyperlink ref="T118" r:id="rId105" display="https://www.ncbi.nlm.nih.gov/pubmed/12226499"/>
+    <hyperlink ref="T126" r:id="rId106" display="https://www.ncbi.nlm.nih.gov/pubmed/21159198"/>
+    <hyperlink ref="T140" r:id="rId107" display="https://www.ncbi.nlm.nih.gov/pubmed/18316719"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId92"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId108"/>
 </worksheet>
 </file>
 

</xml_diff>